<commit_message>
Commiting scripts (R22 UAT2 - Regression).
</commit_message>
<xml_diff>
--- a/Data/Account Statement.xlsx
+++ b/Data/Account Statement.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
   <si>
     <t>Transaction Number</t>
   </si>
@@ -62,7 +62,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -83,6 +83,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>